<commit_message>
Corrected issue with u-USB pinout. Moved USB A connector down a bit for more clearance. Rev 2.0
</commit_message>
<xml_diff>
--- a/onion2 breakout.xlsx
+++ b/onion2 breakout.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
   <si>
     <t>Id</t>
   </si>
@@ -139,13 +139,67 @@
   </si>
   <si>
     <t>Totals:</t>
+  </si>
+  <si>
+    <t>Shipped Date</t>
+  </si>
+  <si>
+    <t>Est delivery</t>
+  </si>
+  <si>
+    <t>Tracking</t>
+  </si>
+  <si>
+    <t>HK05232788AM</t>
+  </si>
+  <si>
+    <t>LK185171893CN</t>
+  </si>
+  <si>
+    <t>3/29-5/5</t>
+  </si>
+  <si>
+    <t>3/29-5/6</t>
+  </si>
+  <si>
+    <t>3/29-5/7</t>
+  </si>
+  <si>
+    <t>3/29-5/8</t>
+  </si>
+  <si>
+    <t>3/29-5/9</t>
+  </si>
+  <si>
+    <t>3/24-4/3</t>
+  </si>
+  <si>
+    <t>Received?</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>3/21-4/6</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>PCB Board 1.57"x2.05</t>
+  </si>
+  <si>
+    <t>OshPark</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,8 +334,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,6 +521,30 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -626,7 +712,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -669,8 +755,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -689,8 +776,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -724,6 +822,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -734,7 +833,28 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1010,10 +1130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,12 +1141,21 @@
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="10" max="10" width="9" customWidth="1"/>
+    <col min="11" max="11" width="1.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1057,8 +1186,21 @@
       <c r="J1" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="K1" s="12"/>
+      <c r="L1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" s="3" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="3" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1091,8 +1233,21 @@
         <f>I2*D2</f>
         <v>0.47899999999999998</v>
       </c>
+      <c r="K2" s="13"/>
+      <c r="L2" s="10">
+        <v>42805</v>
+      </c>
+      <c r="M2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1118,15 +1273,28 @@
         <v>1.69</v>
       </c>
       <c r="I3" s="7">
-        <f t="shared" ref="I3:I12" si="0">H3/G3</f>
+        <f t="shared" ref="I3:I13" si="0">H3/G3</f>
         <v>3.3799999999999997E-2</v>
       </c>
       <c r="J3" s="7">
-        <f t="shared" ref="J3:J12" si="1">I3*D3</f>
+        <f t="shared" ref="J3:J13" si="1">I3*D3</f>
         <v>6.7599999999999993E-2</v>
       </c>
+      <c r="K3" s="13"/>
+      <c r="L3" s="10">
+        <v>42805</v>
+      </c>
+      <c r="M3" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1159,8 +1327,21 @@
         <f t="shared" si="1"/>
         <v>0.13</v>
       </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="10">
+        <v>42805</v>
+      </c>
+      <c r="M4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1193,8 +1374,21 @@
         <f t="shared" si="1"/>
         <v>5.9800000000000006E-2</v>
       </c>
+      <c r="K5" s="13"/>
+      <c r="L5" s="10">
+        <v>42805</v>
+      </c>
+      <c r="M5" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="O5" s="15" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1227,8 +1421,21 @@
         <f t="shared" si="1"/>
         <v>3.3799999999999997E-2</v>
       </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="10">
+        <v>42805</v>
+      </c>
+      <c r="M6" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1261,40 +1468,58 @@
         <f t="shared" si="1"/>
         <v>0.55099999999999993</v>
       </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="14">
+        <v>9.20019017738003E+21</v>
+      </c>
+      <c r="N7" s="10">
+        <v>42812</v>
+      </c>
+      <c r="O7" s="15" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+    <row r="8" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="18">
         <v>2</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7">
+      <c r="F8" s="18"/>
+      <c r="G8" s="18">
         <v>1</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="18">
         <v>0</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1327,8 +1552,17 @@
         <f t="shared" si="1"/>
         <v>0.59899999999999998</v>
       </c>
+      <c r="K9" s="13"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="O9" s="15" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1361,8 +1595,15 @@
         <f t="shared" si="1"/>
         <v>0.495</v>
       </c>
+      <c r="K10" s="13"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="15" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1395,8 +1636,17 @@
         <f t="shared" si="1"/>
         <v>0.28900000000000003</v>
       </c>
+      <c r="K11" s="13"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="10">
+        <v>42812</v>
+      </c>
+      <c r="O11" s="16" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1429,22 +1679,92 @@
         <f t="shared" si="1"/>
         <v>0.23500000000000001</v>
       </c>
+      <c r="K12" s="13"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="O12" s="15" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G14" s="9" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="7">
+        <v>3</v>
+      </c>
+      <c r="H13" s="7">
+        <v>16</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="0"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="1"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="K13" s="13"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="O13" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G16" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="2">
-        <f>SUM(H2:H12)</f>
-        <v>39.350000000000009</v>
-      </c>
-      <c r="J14" s="2">
-        <f>SUM(J2:J12)</f>
-        <v>2.9392</v>
+      <c r="H16" s="2">
+        <f>SUM(H2:H13)</f>
+        <v>55.350000000000009</v>
+      </c>
+      <c r="J16" s="2">
+        <f>SUM(J2:J13)</f>
+        <v>8.2725333333333335</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="O2:O13">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="F">
+      <formula>NOT(ISERROR(SEARCH("F",O2)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="M7" r:id="rId1" tooltip="Tracking number" display="javascript:;"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>